<commit_message>
Update forum2023.md: ajout intervenant
</commit_message>
<xml_diff>
--- a/static/documents/planning_forum_2023.xlsx
+++ b/static/documents/planning_forum_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Programmation\Github\prepas-mp2i.fr\static\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66ACBCE4-E8AB-4F19-992F-00221BA2BF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADDDD8D-E39D-40F3-A9A8-C508476B5489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{538145DD-04CD-4D5C-B440-70EC89FD71D2}"/>
   </bookViews>
@@ -16,29 +16,19 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$F$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$F$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Ville</t>
   </si>
@@ -137,6 +127,12 @@
   </si>
   <si>
     <t>14h-14h55</t>
+  </si>
+  <si>
+    <t>Bordeaux - 33</t>
+  </si>
+  <si>
+    <t>Montaigne</t>
   </si>
 </sst>
 </file>
@@ -444,33 +440,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -515,46 +505,51 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -883,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1CB0AB-5AF2-4B03-90C3-4D2EBFD9C2ED}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,24 +891,24 @@
     <col min="3" max="6" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36"/>
+    </row>
+    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
       <c r="B2" s="33"/>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="27" t="s">
         <v>32</v>
       </c>
       <c r="D2" s="6" t="s">
@@ -922,18 +917,18 @@
       <c r="E2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="28" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+    <row r="3" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>1</v>
       </c>
       <c r="D3" s="7">
@@ -942,19 +937,18 @@
       <c r="E3" s="7">
         <v>6</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="13">
         <v>5</v>
       </c>
-      <c r="G3" s="37"/>
-    </row>
-    <row r="4" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+    </row>
+    <row r="4" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <v>1</v>
       </c>
       <c r="D4" s="1">
@@ -963,18 +957,18 @@
       <c r="E4" s="2">
         <v>6</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+    <row r="5" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>2</v>
       </c>
       <c r="D5" s="3">
@@ -983,18 +977,18 @@
       <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>2</v>
       </c>
       <c r="D6" s="3">
@@ -1003,136 +997,136 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="12">
-        <v>3</v>
+    <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="13">
+    <row r="8" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="10">
         <v>3</v>
       </c>
-      <c r="D8" s="2">
-        <v>3</v>
+      <c r="D8" s="3">
+        <v>2</v>
       </c>
       <c r="E8" s="3">
         <v>2</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="15">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+    <row r="9" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="11">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B10" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C10" s="10">
         <v>4</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D10" s="4">
         <v>3</v>
-      </c>
-      <c r="E9" s="4">
-        <v>3</v>
-      </c>
-      <c r="F9" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="14">
-        <v>4</v>
-      </c>
-      <c r="D10" s="2">
-        <v>4</v>
       </c>
       <c r="E10" s="4">
         <v>3</v>
       </c>
-      <c r="F10" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="14">
-        <v>5</v>
+      <c r="F10" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="12">
+        <v>4</v>
       </c>
       <c r="D11" s="2">
         <v>4</v>
       </c>
       <c r="E11" s="4">
+        <v>3</v>
+      </c>
+      <c r="F11" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="12">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
         <v>4</v>
       </c>
-      <c r="F11" s="19">
+      <c r="E12" s="4">
+        <v>4</v>
+      </c>
+      <c r="F12" s="17">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+    <row r="13" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B13" s="22" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" s="14">
-        <v>5</v>
-      </c>
-      <c r="D12" s="5">
-        <v>5</v>
-      </c>
-      <c r="E12" s="5">
-        <v>4</v>
-      </c>
-      <c r="F12" s="16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>24</v>
       </c>
       <c r="C13" s="12">
         <v>5</v>
@@ -1141,54 +1135,71 @@
         <v>5</v>
       </c>
       <c r="E13" s="5">
+        <v>4</v>
+      </c>
+      <c r="F13" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="10">
         <v>5</v>
       </c>
-      <c r="F13" s="20">
+      <c r="D14" s="5">
+        <v>5</v>
+      </c>
+      <c r="E14" s="5">
+        <v>5</v>
+      </c>
+      <c r="F14" s="18">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+    <row r="15" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C15" s="10">
         <v>6</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D15" s="4">
         <v>5</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E15" s="4">
         <v>5</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F15" s="17">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+    <row r="16" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B16" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C16" s="19">
         <v>6</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D16" s="20">
         <v>6</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E16" s="20">
         <v>5</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F16" s="21">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F16" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1197,7 +1208,7 @@
     <mergeCell ref="C1:F1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C3:F15">
+  <conditionalFormatting sqref="C3:F16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1263,7 +1274,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:F15">
+  <conditionalFormatting sqref="A3:F16">
     <cfRule type="colorScale" priority="144">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>